<commit_message>
merge removed from excel
</commit_message>
<xml_diff>
--- a/screaper_backend/resources/templates/BMTemplate_202103.xlsx
+++ b/screaper_backend/resources/templates/BMTemplate_202103.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/screaper/screaper_backend/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{90D00DBA-7E20-5349-8430-EEAAD3734FC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{46A6FF34-25F6-FE48-A859-CCFC471B7241}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
@@ -728,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -877,9 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="198" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1729,7 +1726,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -1748,34 +1745,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="79"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="A1" s="78"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
     </row>
     <row r="3" spans="1:10" ht="21.5" customHeight="1">
-      <c r="A3" s="79"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
+      <c r="A3" s="78"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
     </row>
     <row r="4" spans="1:10" ht="33.5" customHeight="1">
       <c r="A4" s="71" t="s">
@@ -1792,7 +1789,7 @@
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="79" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="75"/>
@@ -1848,14 +1845,14 @@
       <c r="J8" s="23"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A9" s="78"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
     </row>
@@ -1870,7 +1867,7 @@
       <c r="F10" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="95">
+      <c r="H10" s="94">
         <v>44259</v>
       </c>
     </row>
@@ -1885,7 +1882,7 @@
       <c r="F11" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="95">
+      <c r="H11" s="94">
         <v>44258</v>
       </c>
     </row>
@@ -1895,11 +1892,11 @@
       <c r="C12" s="67"/>
       <c r="D12" s="67"/>
       <c r="E12" s="67"/>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A13" s="26" t="s">
@@ -1930,11 +1927,11 @@
       <c r="C15" s="26"/>
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
-      <c r="F15" s="81" t="s">
+      <c r="F15" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="7.25" customHeight="1">
@@ -1982,10 +1979,10 @@
       <c r="F18" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G18" s="85" t="s">
+      <c r="G18" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="83"/>
+      <c r="H18" s="82"/>
       <c r="K18" s="25" t="s">
         <v>12</v>
       </c>
@@ -2013,8 +2010,8 @@
       <c r="F19" s="70">
         <v>181.4</v>
       </c>
-      <c r="G19" s="86"/>
-      <c r="H19" s="87">
+      <c r="G19" s="85"/>
+      <c r="H19" s="86">
         <f>F19*B19</f>
         <v>362.8</v>
       </c>
@@ -2035,8 +2032,8 @@
       <c r="D20" s="33"/>
       <c r="E20" s="68"/>
       <c r="F20" s="66"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="88"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="87"/>
       <c r="K20" s="53"/>
       <c r="L20" s="53"/>
       <c r="M20" s="3"/>
@@ -2048,8 +2045,8 @@
       <c r="D21" s="35"/>
       <c r="E21" s="36"/>
       <c r="F21" s="37"/>
-      <c r="G21" s="102"/>
-      <c r="H21" s="102"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
       <c r="K21" s="8"/>
@@ -2061,12 +2058,12 @@
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
       <c r="D22" s="35"/>
-      <c r="E22" s="96" t="s">
+      <c r="E22" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="97"/>
-      <c r="G22" s="89"/>
-      <c r="H22" s="90">
+      <c r="F22" s="96"/>
+      <c r="G22" s="88"/>
+      <c r="H22" s="89">
         <v>0</v>
       </c>
       <c r="I22" s="11"/>
@@ -2080,12 +2077,12 @@
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
       <c r="D23" s="35"/>
-      <c r="E23" s="98" t="s">
+      <c r="E23" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="F23" s="99"/>
-      <c r="G23" s="91"/>
-      <c r="H23" s="92">
+      <c r="F23" s="98"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="91">
         <v>0</v>
       </c>
       <c r="I23" s="9"/>
@@ -2099,12 +2096,12 @@
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
       <c r="D24" s="35"/>
-      <c r="E24" s="100" t="s">
+      <c r="E24" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="101"/>
-      <c r="G24" s="93"/>
-      <c r="H24" s="94">
+      <c r="F24" s="100"/>
+      <c r="G24" s="92"/>
+      <c r="H24" s="93">
         <v>0</v>
       </c>
       <c r="I24" s="9"/>
@@ -2120,8 +2117,8 @@
       <c r="D25" s="35"/>
       <c r="E25" s="38"/>
       <c r="F25" s="37"/>
-      <c r="G25" s="77"/>
-      <c r="H25" s="77"/>
+      <c r="G25" s="101"/>
+      <c r="H25" s="101"/>
       <c r="I25" s="20"/>
       <c r="J25" s="11"/>
       <c r="K25" s="11"/>
@@ -2327,11 +2324,11 @@
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
-      <c r="F42" s="81" t="s">
+      <c r="F42" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="81"/>
-      <c r="H42" s="81"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="14"/>
@@ -2398,9 +2395,9 @@
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="82"/>
+      <c r="F50" s="81"/>
+      <c r="G50" s="81"/>
+      <c r="H50" s="81"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="1"/>
@@ -2415,9 +2412,8 @@
       <c r="H54" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="15">
     <mergeCell ref="F50:H50"/>
-    <mergeCell ref="G25:H25"/>
     <mergeCell ref="F42:H42"/>
     <mergeCell ref="A1:H3"/>
     <mergeCell ref="A6:H6"/>

</xml_diff>